<commit_message>
Remove os from skills
</commit_message>
<xml_diff>
--- a/downloads/skillsNasahl.xlsx
+++ b/downloads/skillsNasahl.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Homepage\website-nasahl\skills\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Homepage\website-nasahl\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D8C26C-3392-4421-BA01-63861BD41613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E24BBD1-18A0-4EE9-8624-AB8740A2E399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67080" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{FFED163B-1A79-4166-8907-A941EF55E520}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FFED163B-1A79-4166-8907-A941EF55E520}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="87">
   <si>
     <t>Methodik</t>
   </si>
@@ -282,7 +282,10 @@
     <t>Aktualisiert</t>
   </si>
   <si>
-    <t>26.10.2023</t>
+    <t>Betriebssystem</t>
+  </si>
+  <si>
+    <t>03.11.2023</t>
   </si>
 </sst>
 </file>
@@ -654,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A1FE19F-B544-42DE-B99C-7467554A9C25}">
-  <dimension ref="A1:D97"/>
+  <dimension ref="A1:D98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -677,7 +680,7 @@
         <v>84</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -1020,58 +1023,58 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C54" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C55" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="C56" s="3">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="D56" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C57" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C58" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C59" s="3">
-        <v>2</v>
-      </c>
-      <c r="D59" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C60" s="3">
         <v>3</v>
@@ -1079,7 +1082,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C61" s="3">
         <v>4</v>
@@ -1087,15 +1090,15 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C62" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C63" s="3">
         <v>3</v>
@@ -1103,71 +1106,71 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C64" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B65" t="s">
-        <v>48</v>
-      </c>
-      <c r="C65" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B66" t="s">
-        <v>49</v>
-      </c>
-      <c r="C66" s="3">
-        <v>3</v>
+      <c r="A66" t="s">
+        <v>8</v>
+      </c>
+      <c r="D66" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C67" s="3">
-        <v>3</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B68" t="s">
+        <v>59</v>
+      </c>
+      <c r="C68" s="3">
+        <v>4</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>8</v>
-      </c>
-      <c r="D69" s="3">
-        <v>0</v>
+      <c r="B69" t="s">
+        <v>60</v>
+      </c>
+      <c r="C69" s="3">
+        <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C70" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="C71" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="C72" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C73" s="3">
         <v>3</v>
@@ -1175,7 +1178,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C74" s="3">
         <v>3</v>
@@ -1183,7 +1186,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="C75" s="3">
         <v>3</v>
@@ -1191,7 +1194,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C76" s="3">
         <v>3</v>
@@ -1199,7 +1202,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C77" s="3">
         <v>3</v>
@@ -1207,7 +1210,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="C78" s="3">
         <v>3</v>
@@ -1215,7 +1218,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="C79" s="3">
         <v>3</v>
@@ -1223,115 +1226,123 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C80" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="C81" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B82" t="s">
-        <v>36</v>
-      </c>
-      <c r="C82" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B83" t="s">
-        <v>67</v>
-      </c>
-      <c r="C83" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>85</v>
+      </c>
+      <c r="D83" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="C84" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B85" t="s">
+        <v>52</v>
+      </c>
+      <c r="C85" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B86" t="s">
+        <v>74</v>
+      </c>
+      <c r="C86" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B88" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B89" t="s">
         <v>54</v>
-      </c>
-      <c r="C88" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B89" t="s">
-        <v>55</v>
       </c>
       <c r="C89" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
+        <v>55</v>
+      </c>
+      <c r="C90" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B91" t="s">
         <v>77</v>
       </c>
-      <c r="C90" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B91" t="s">
+      <c r="C91" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B92" t="s">
         <v>56</v>
       </c>
-      <c r="C91" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B92" t="s">
+      <c r="C92" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B93" t="s">
         <v>57</v>
       </c>
-      <c r="C92" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
+      <c r="C93" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B95" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B96" t="s">
         <v>69</v>
       </c>
-      <c r="C95" s="3">
+      <c r="C96" s="3">
         <v>5</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B96" t="s">
-        <v>70</v>
-      </c>
-      <c r="C96" s="3">
-        <v>3</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B97" t="s">
+        <v>70</v>
+      </c>
+      <c r="C97" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B98" t="s">
         <v>71</v>
       </c>
-      <c r="C97" s="3">
+      <c r="C98" s="3">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adapt skill OAuth2 / OpenID Connect
</commit_message>
<xml_diff>
--- a/downloads/skillsNasahl.xlsx
+++ b/downloads/skillsNasahl.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Homepage\website-nasahl\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B31A0CBC-06A5-4F07-BDCB-947BA3BEAA0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836FE368-23A1-4085-9FA9-E349E0CA6F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67080" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{FFED163B-1A79-4166-8907-A941EF55E520}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FFED163B-1A79-4166-8907-A941EF55E520}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="90">
   <si>
     <t>Methodik</t>
   </si>
@@ -292,6 +292,9 @@
   </si>
   <si>
     <t>RabbitMQ</t>
+  </si>
+  <si>
+    <t>OAuth2/OpenID Connect</t>
   </si>
 </sst>
 </file>
@@ -663,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A1FE19F-B544-42DE-B99C-7467554A9C25}">
-  <dimension ref="A1:D100"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -901,7 +904,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="C36" s="3">
         <v>3</v>
@@ -909,31 +912,31 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C37" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="C38" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C39" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C40" s="3">
         <v>2</v>
@@ -941,63 +944,63 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C41" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
       <c r="C42" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>24</v>
+        <v>88</v>
       </c>
       <c r="C43" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>87</v>
+        <v>24</v>
       </c>
       <c r="C44" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
+        <v>87</v>
+      </c>
+      <c r="C45" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
         <v>23</v>
       </c>
-      <c r="C45" s="3">
-        <v>4</v>
-      </c>
-      <c r="D45" s="3">
+      <c r="C46" s="3">
+        <v>4</v>
+      </c>
+      <c r="D46" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B48" t="s">
-        <v>33</v>
-      </c>
-      <c r="C48" s="3">
-        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C49" s="3">
         <v>4</v>
@@ -1005,98 +1008,98 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C50" s="3">
-        <v>2</v>
-      </c>
-      <c r="D50" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C51" s="3">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="D51" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C52" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
+        <v>37</v>
+      </c>
+      <c r="C53" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
         <v>38</v>
       </c>
-      <c r="C53" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+      <c r="C54" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B56" t="s">
-        <v>40</v>
-      </c>
-      <c r="C56" s="3">
-        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C57" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C58" s="3">
-        <v>2</v>
-      </c>
-      <c r="D58" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C59" s="3">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="D59" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C60" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C61" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C62" s="3">
         <v>3</v>
@@ -1104,15 +1107,15 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C63" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C64" s="3">
         <v>4</v>
@@ -1120,39 +1123,39 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C65" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
+        <v>49</v>
+      </c>
+      <c r="C66" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
         <v>50</v>
       </c>
-      <c r="C66" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+      <c r="C67" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>8</v>
       </c>
-      <c r="D68" s="3">
+      <c r="D69" s="3">
         <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B69" t="s">
-        <v>58</v>
-      </c>
-      <c r="C69" s="3">
-        <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C70" s="3">
         <v>4</v>
@@ -1160,7 +1163,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C71" s="3">
         <v>4</v>
@@ -1168,15 +1171,15 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C72" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="C73" s="3">
         <v>3</v>
@@ -1184,7 +1187,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C74" s="3">
         <v>3</v>
@@ -1192,7 +1195,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="C75" s="3">
         <v>3</v>
@@ -1200,7 +1203,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C76" s="3">
         <v>3</v>
@@ -1208,7 +1211,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C77" s="3">
         <v>3</v>
@@ -1216,7 +1219,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C78" s="3">
         <v>3</v>
@@ -1224,7 +1227,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C79" s="3">
         <v>3</v>
@@ -1232,7 +1235,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="C80" s="3">
         <v>3</v>
@@ -1240,7 +1243,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C81" s="3">
         <v>3</v>
@@ -1248,7 +1251,7 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="C82" s="3">
         <v>3</v>
@@ -1256,60 +1259,60 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
+        <v>67</v>
+      </c>
+      <c r="C83" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B84" t="s">
         <v>68</v>
       </c>
-      <c r="C83" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
+      <c r="C84" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
         <v>85</v>
       </c>
-      <c r="D85" s="3">
+      <c r="D86" s="3">
         <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B86" t="s">
-        <v>51</v>
-      </c>
-      <c r="C86" s="3">
-        <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B87" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C87" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
+        <v>52</v>
+      </c>
+      <c r="C88" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B89" t="s">
         <v>74</v>
       </c>
-      <c r="C88" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
+      <c r="C89" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B91" t="s">
-        <v>54</v>
-      </c>
-      <c r="C91" s="3">
-        <v>5</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C92" s="3">
         <v>5</v>
@@ -1317,15 +1320,15 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="C93" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B94" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="C94" s="3">
         <v>4</v>
@@ -1333,38 +1336,46 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B95" t="s">
+        <v>56</v>
+      </c>
+      <c r="C95" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B96" t="s">
         <v>57</v>
       </c>
-      <c r="C95" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
+      <c r="C96" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B98" t="s">
-        <v>69</v>
-      </c>
-      <c r="C98" s="3">
-        <v>5</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B99" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C99" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
+        <v>70</v>
+      </c>
+      <c r="C100" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B101" t="s">
         <v>71</v>
       </c>
-      <c r="C100" s="3">
+      <c r="C101" s="3">
         <v>3</v>
       </c>
     </row>

</xml_diff>